<commit_message>
update general + add vote system (borda.count)
</commit_message>
<xml_diff>
--- a/notebooks/assets/test/RF10_01.xlsx
+++ b/notebooks/assets/test/RF10_01.xlsx
@@ -467,19 +467,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.126</v>
+        <v>0.214</v>
       </c>
       <c r="C2" t="n">
-        <v>0.177</v>
+        <v>0.246</v>
       </c>
       <c r="D2" t="n">
-        <v>0.137</v>
+        <v>0.173</v>
       </c>
       <c r="E2" t="n">
-        <v>0.259</v>
+        <v>0.314</v>
       </c>
       <c r="F2" t="n">
-        <v>0.14</v>
+        <v>0.256</v>
       </c>
     </row>
     <row r="3">
@@ -489,19 +489,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.039</v>
+        <v>0.18</v>
       </c>
       <c r="C3" t="n">
-        <v>0.175</v>
+        <v>0.171</v>
       </c>
       <c r="D3" t="n">
-        <v>0.059</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="E3" t="n">
-        <v>0.217</v>
+        <v>0.543</v>
       </c>
       <c r="F3" t="n">
-        <v>0.046</v>
+        <v>0.198</v>
       </c>
     </row>
     <row r="4">
@@ -533,19 +533,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>18.294</v>
+        <v>18.285</v>
       </c>
       <c r="C5" t="n">
-        <v>15.308</v>
+        <v>15.301</v>
       </c>
       <c r="D5" t="n">
-        <v>13.168</v>
+        <v>13.131</v>
       </c>
       <c r="E5" t="n">
-        <v>31.158</v>
+        <v>31.133</v>
       </c>
       <c r="F5" t="n">
-        <v>18.206</v>
+        <v>18.158</v>
       </c>
     </row>
     <row r="6">
@@ -555,19 +555,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.996</v>
+        <v>0.981</v>
       </c>
       <c r="C6" t="n">
         <v>0.987</v>
       </c>
       <c r="D6" t="n">
-        <v>0.983</v>
+        <v>0.975</v>
       </c>
       <c r="E6" t="n">
-        <v>0.995</v>
+        <v>0.987</v>
       </c>
       <c r="F6" t="n">
-        <v>0.998</v>
+        <v>0.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>